<commit_message>
rafactor master data related code
</commit_message>
<xml_diff>
--- a/client/Assets/StreamingAssets/MasterData/MasterData.xlsx
+++ b/client/Assets/StreamingAssets/MasterData/MasterData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myoshida\AppData\LocalLow\DefaultCompany\client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myoshida\dev\genie\client\Assets\StreamingAssets\MasterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8031D917-0D7A-478D-AE8F-F6B627BCF773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82391D4E-DEE6-4FC9-94FD-9EA872A8464F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30585" yWindow="615" windowWidth="21600" windowHeight="11295" xr2:uid="{87C9C6BE-52D2-40D4-B4AF-044D8B0A8C86}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{87C9C6BE-52D2-40D4-B4AF-044D8B0A8C86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,10 +42,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>CharacterMaster</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Code</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -139,6 +135,10 @@
   </si>
   <si>
     <t>SimpleNaturePack/Prefabs/Ground_01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PlayerMaster</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -534,7 +534,7 @@
   <dimension ref="A2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -551,30 +551,30 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -582,10 +582,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -605,10 +605,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -628,10 +628,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -651,27 +651,27 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
       <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -679,10 +679,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -694,24 +694,24 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
@@ -719,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -736,7 +736,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -753,7 +753,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>1</v>

</xml_diff>

<commit_message>
put player through lua
</commit_message>
<xml_diff>
--- a/client/Assets/StreamingAssets/MasterData/MasterData.xlsx
+++ b/client/Assets/StreamingAssets/MasterData/MasterData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myoshida\dev\genie\client\Assets\StreamingAssets\MasterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82391D4E-DEE6-4FC9-94FD-9EA872A8464F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4F86C0-FA04-41E7-A7B4-6020E2FABF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{87C9C6BE-52D2-40D4-B4AF-044D8B0A8C86}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="A2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -588,7 +588,7 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>1</v>

</xml_diff>

<commit_message>
object master with rock, mushrrom
</commit_message>
<xml_diff>
--- a/client/Assets/StreamingAssets/MasterData/MasterData.xlsx
+++ b/client/Assets/StreamingAssets/MasterData/MasterData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myoshida\dev\genie\client\Assets\StreamingAssets\MasterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4F86C0-FA04-41E7-A7B4-6020E2FABF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151593F2-24A6-49CB-83C4-2BAB64D1FC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{87C9C6BE-52D2-40D4-B4AF-044D8B0A8C86}"/>
+    <workbookView xWindow="31620" yWindow="1650" windowWidth="21600" windowHeight="11295" xr2:uid="{87C9C6BE-52D2-40D4-B4AF-044D8B0A8C86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>MASTERDATA</t>
     <phoneticPr fontId="1"/>
@@ -139,6 +139,26 @@
   </si>
   <si>
     <t>PlayerMaster</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ObjectMaster</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ObjectType</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rock</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SimpleNaturePack/Prefabs/Rock_05</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mushroom</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -531,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F28025-8CED-4B64-B095-19EECE0C87D8}">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A2:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -651,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -659,19 +679,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -679,93 +699,160 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14">
-        <v>1</v>
+      <c r="A14" t="s">
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B22" t="s">
         <v>17</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
         <v>2</v>
       </c>
     </row>
-    <row r="17" customFormat="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>